<commit_message>
[Pipette] Transformer 구조 update
</commit_message>
<xml_diff>
--- a/4_Transformer/1_Schematic/V2.0/Plasma_Gen_Transformer_Part List_V2.0.xlsx
+++ b/4_Transformer/1_Schematic/V2.0/Plasma_Gen_Transformer_Part List_V2.0.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Work\20171116_Plasma_Generator\4_Transformer\1_Schematic\V2.0\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="28035" windowHeight="12780"/>
   </bookViews>
   <sheets>
     <sheet name="Plasma_Gen_Transformer_SCH_V2.0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="79">
   <si>
     <t>No</t>
   </si>
@@ -254,6 +259,22 @@
   </si>
   <si>
     <t>Type C</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>053261-0571</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.25mm Pitch Header, Surface Mount, Right Angle, 5-Pin</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>053048-0510</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.25mm Pitch Header, Thru-Hole, Right Angle, 5-Pin</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -1421,6 +1442,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1468,7 +1492,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1503,7 +1527,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1712,10 +1736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R17"/>
+  <dimension ref="B1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2299,7 +2323,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="17" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="J17" s="22">
         <f>SUM(J15:J16)</f>
         <v>280</v>
@@ -2307,6 +2331,28 @@
       <c r="L17" s="22">
         <f>SUM(L15:L16)</f>
         <v>4000</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Pipette] Transformer SCH update
</commit_message>
<xml_diff>
--- a/4_Transformer/1_Schematic/V2.0/Plasma_Gen_Transformer_Part List_V2.0.xlsx
+++ b/4_Transformer/1_Schematic/V2.0/Plasma_Gen_Transformer_Part List_V2.0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="16155" windowHeight="9180"/>
@@ -12,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Plasma_Transformer_V2.0!$B$5:$L$5</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="83">
   <si>
     <t>No</t>
   </si>
@@ -127,13 +127,7 @@
     <t>NVMFS5C450NL</t>
   </si>
   <si>
-    <t>NTD5802N</t>
-  </si>
-  <si>
     <t>ON Semiconductor</t>
-  </si>
-  <si>
-    <t>Power MOSFET 40V, Single N-Channel, 101A DPAK</t>
   </si>
   <si>
     <t>Q1,Q2</t>
@@ -262,19 +256,23 @@
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
+    <t>P007567011</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>053398-0571</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>P005634282</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
     <t>NVMFS5C450NL</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>P007567011</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
-    <t>053398-0571</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
-    <t>P005634282</t>
+    <t>40V, 2.8mOhm , 110A, Single N−Channel Power MOSFET</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -1627,7 +1625,7 @@
   <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1649,12 +1647,12 @@
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="P3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1700,28 +1698,28 @@
         <v>10</v>
       </c>
       <c r="M5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="N5" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="O5" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="P5" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="N5" s="25" t="s">
+      <c r="Q5" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="O5" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="P5" s="27" t="s">
+      <c r="R5" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="Q5" s="27" t="s">
+      <c r="S5" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="R5" s="27" t="s">
+      <c r="T5" s="35" t="s">
         <v>74</v>
-      </c>
-      <c r="S5" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="T5" s="35" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
@@ -1772,14 +1770,14 @@
         <v>40</v>
       </c>
       <c r="P6" s="30">
-        <f>H6*$P$4</f>
+        <f t="shared" ref="P6:P12" si="0">H6*$P$4</f>
         <v>10</v>
       </c>
       <c r="Q6" s="28"/>
       <c r="R6" s="28"/>
       <c r="S6" s="37"/>
       <c r="T6" s="29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
@@ -1823,19 +1821,19 @@
         <v>10</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" ref="N7:N14" si="0">H7*M7</f>
+        <f t="shared" ref="N7:N14" si="1">H7*M7</f>
         <v>20</v>
       </c>
       <c r="O7" s="20"/>
       <c r="P7" s="31">
-        <f>H7*$P$4</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="Q7" s="20"/>
       <c r="R7" s="20"/>
       <c r="S7" s="38"/>
       <c r="T7" s="33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
@@ -1877,19 +1875,19 @@
         <v>10</v>
       </c>
       <c r="N8" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="O8" s="20"/>
       <c r="P8" s="31">
-        <f>H8*$P$4</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="Q8" s="20"/>
       <c r="R8" s="20"/>
       <c r="S8" s="38"/>
       <c r="T8" s="33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
@@ -1900,31 +1898,31 @@
         <v>4</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D9" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>37</v>
-      </c>
       <c r="F9" s="16" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="H9" s="16">
         <v>2</v>
       </c>
       <c r="I9" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="16" t="s">
-        <v>41</v>
-      </c>
       <c r="K9" s="16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L9" s="16" t="s">
         <v>35</v>
@@ -1933,14 +1931,14 @@
         <v>1020</v>
       </c>
       <c r="N9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2040</v>
       </c>
       <c r="O9" s="16">
         <v>4</v>
       </c>
       <c r="P9" s="31">
-        <f>H9*$P$4</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="Q9" s="16">
@@ -1954,7 +1952,7 @@
         <v>20400</v>
       </c>
       <c r="T9" s="36" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
@@ -1965,47 +1963,47 @@
         <v>5</v>
       </c>
       <c r="C10" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="16" t="s">
         <v>42</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>44</v>
       </c>
       <c r="H10" s="16">
         <v>1</v>
       </c>
       <c r="I10" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="16" t="s">
-        <v>47</v>
-      </c>
       <c r="K10" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M10" s="16">
         <v>130</v>
       </c>
       <c r="N10" s="4">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="O10" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="P10" s="31">
         <f t="shared" si="0"/>
-        <v>130</v>
-      </c>
-      <c r="O10" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="P10" s="31">
-        <f>H10*$P$4</f>
         <v>10</v>
       </c>
       <c r="Q10" s="16">
@@ -2019,7 +2017,7 @@
         <v>13000</v>
       </c>
       <c r="T10" s="36" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
@@ -2030,47 +2028,47 @@
         <v>8</v>
       </c>
       <c r="C11" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="F11" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="16" t="s">
         <v>56</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>58</v>
       </c>
       <c r="H11" s="16">
         <v>1</v>
       </c>
       <c r="I11" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="J11" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="J11" s="16" t="s">
-        <v>61</v>
-      </c>
       <c r="K11" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M11" s="16">
         <v>160</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>160</v>
       </c>
       <c r="O11" s="20">
         <v>50</v>
       </c>
       <c r="P11" s="20">
-        <f>H11*$P$4</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="Q11" s="20"/>
@@ -2086,45 +2084,45 @@
         <v>9</v>
       </c>
       <c r="C12" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="16" t="s">
         <v>62</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>64</v>
       </c>
       <c r="H12" s="16">
         <v>1</v>
       </c>
       <c r="I12" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="J12" s="16" t="s">
-        <v>67</v>
-      </c>
       <c r="K12" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M12" s="14">
         <v>10000</v>
       </c>
       <c r="N12" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10000</v>
       </c>
       <c r="O12" s="20"/>
       <c r="P12" s="20">
-        <f>H12*$P$4</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="Q12" s="20"/>
@@ -2134,38 +2132,38 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B13" s="19">
         <v>6</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H13" s="20">
         <v>1</v>
       </c>
       <c r="I13" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K13" s="20"/>
       <c r="L13" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M13" s="20">
         <v>0</v>
       </c>
       <c r="N13" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O13" s="20"/>
@@ -2177,13 +2175,13 @@
     </row>
     <row r="14" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B14" s="22">
         <v>7</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
@@ -2193,20 +2191,20 @@
         <v>4</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J14" s="17">
         <v>0</v>
       </c>
       <c r="K14" s="17"/>
       <c r="L14" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M14" s="17">
         <v>0</v>
       </c>
       <c r="N14" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O14" s="17"/>
@@ -2228,7 +2226,7 @@
     </row>
     <row r="16" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>